<commit_message>
add flag gotolast 2
</commit_message>
<xml_diff>
--- a/Information/Изменение результатов.xlsx
+++ b/Information/Изменение результатов.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\диплом\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\MAPF_System\Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47420463-4DD6-411B-9452-6B43CE3F38BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F228D8C-4BD4-4C98-AA0C-7FD0319CC164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BBE610F-FD71-401D-9DCE-6AF9F6A4B4C0}"/>
   </bookViews>
@@ -859,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +878,7 @@
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -919,7 +919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -959,9 +959,8 @@
       <c r="M2" s="3">
         <v>7</v>
       </c>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1001,9 +1000,8 @@
       <c r="M3" s="4">
         <v>3</v>
       </c>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -1023,9 +1021,8 @@
       <c r="M4" s="5">
         <v>43</v>
       </c>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1065,9 +1062,8 @@
       <c r="M5" s="4">
         <v>22</v>
       </c>
-      <c r="N5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1107,9 +1103,8 @@
       <c r="M6" s="3">
         <v>3</v>
       </c>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1149,9 +1144,8 @@
       <c r="M7" s="4">
         <v>8</v>
       </c>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1191,9 +1185,8 @@
       <c r="M8" s="3">
         <v>15</v>
       </c>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1230,12 +1223,11 @@
       <c r="L9" s="4">
         <v>82</v>
       </c>
-      <c r="M9" s="4">
-        <v>82</v>
-      </c>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1275,9 +1267,8 @@
       <c r="M10" s="3">
         <v>67</v>
       </c>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1317,9 +1308,8 @@
       <c r="M11" s="4">
         <v>413</v>
       </c>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1359,9 +1349,8 @@
       <c r="M12" s="3">
         <v>155</v>
       </c>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1401,9 +1390,8 @@
       <c r="M13" s="4">
         <v>147</v>
       </c>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1440,12 +1428,11 @@
       <c r="L14" s="3">
         <v>426</v>
       </c>
-      <c r="M14" s="3">
-        <v>422</v>
-      </c>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M14" s="5">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1485,9 +1472,8 @@
       <c r="M15" s="4">
         <v>128</v>
       </c>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1527,9 +1513,8 @@
       <c r="M16" s="3">
         <v>59</v>
       </c>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1569,9 +1554,8 @@
       <c r="M17" s="6">
         <v>68</v>
       </c>
-      <c r="N17" s="4"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1611,9 +1595,8 @@
       <c r="M18" s="3">
         <v>62</v>
       </c>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -1647,9 +1630,8 @@
       <c r="M19" s="4">
         <v>50</v>
       </c>
-      <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -1683,9 +1665,8 @@
       <c r="M20" s="3">
         <v>50</v>
       </c>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1725,9 +1706,8 @@
       <c r="M21" s="4">
         <v>48</v>
       </c>
-      <c r="N21" s="4"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1767,9 +1747,8 @@
       <c r="M22" s="3">
         <v>43</v>
       </c>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1809,9 +1788,8 @@
       <c r="M23" s="4">
         <v>96</v>
       </c>
-      <c r="N23" s="4"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1851,9 +1829,8 @@
       <c r="M24" s="3">
         <v>18</v>
       </c>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1893,9 +1870,8 @@
       <c r="M25" s="4">
         <v>15</v>
       </c>
-      <c r="N25" s="4"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1935,9 +1911,8 @@
       <c r="M26" s="3">
         <v>51</v>
       </c>
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1977,9 +1952,8 @@
       <c r="M27" s="4">
         <v>32</v>
       </c>
-      <c r="N27" s="4"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2019,9 +1993,8 @@
       <c r="M28" s="3">
         <v>69</v>
       </c>
-      <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2061,9 +2034,8 @@
       <c r="M29" s="8">
         <v>73</v>
       </c>
-      <c r="N29" s="4"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
@@ -2091,9 +2063,8 @@
       <c r="M30" s="3">
         <v>105</v>
       </c>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -2133,9 +2104,8 @@
       <c r="M31" s="4">
         <v>102</v>
       </c>
-      <c r="N31" s="4"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -2175,9 +2145,8 @@
       <c r="M32" s="3">
         <v>16</v>
       </c>
-      <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -2217,9 +2186,8 @@
       <c r="M33" s="6">
         <v>13</v>
       </c>
-      <c r="N33" s="4"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -2259,9 +2227,8 @@
       <c r="M34" s="7">
         <v>13</v>
       </c>
-      <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -2301,9 +2268,8 @@
       <c r="M35" s="6">
         <v>16</v>
       </c>
-      <c r="N35" s="4"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -2343,9 +2309,8 @@
       <c r="M36" s="7">
         <v>16</v>
       </c>
-      <c r="N36" s="3"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -2385,9 +2350,8 @@
       <c r="M37" s="6">
         <v>18</v>
       </c>
-      <c r="N37" s="4"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -2427,9 +2391,8 @@
       <c r="M38" s="7">
         <v>18</v>
       </c>
-      <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -2469,9 +2432,8 @@
       <c r="M39" s="4">
         <v>20</v>
       </c>
-      <c r="N39" s="4"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -2511,9 +2473,8 @@
       <c r="M40" s="3">
         <v>6</v>
       </c>
-      <c r="N40" s="3"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -2553,9 +2514,8 @@
       <c r="M41" s="4">
         <v>10</v>
       </c>
-      <c r="N41" s="4"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -2595,9 +2555,8 @@
       <c r="M42" s="3">
         <v>12</v>
       </c>
-      <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -2637,9 +2596,8 @@
       <c r="M43" s="4">
         <v>15</v>
       </c>
-      <c r="N43" s="4"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>105</v>
       </c>
@@ -2657,9 +2615,8 @@
       <c r="M44" s="7">
         <v>23</v>
       </c>
-      <c r="N44" s="3"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>40</v>
       </c>
@@ -2699,7 +2656,6 @@
       <c r="M45" s="4">
         <v>27</v>
       </c>
-      <c r="N45" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new and delete block function
</commit_message>
<xml_diff>
--- a/Information/Изменение результатов.xlsx
+++ b/Information/Изменение результатов.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\MAPF_System\Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F228D8C-4BD4-4C98-AA0C-7FD0319CC164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33D8CC-AACC-492F-ACCE-62681A93E8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BBE610F-FD71-401D-9DCE-6AF9F6A4B4C0}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
did the correct work with was_near_end
</commit_message>
<xml_diff>
--- a/Information/Изменение результатов.xlsx
+++ b/Information/Изменение результатов.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\MAPF_System\Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B33D8CC-AACC-492F-ACCE-62681A93E8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E86DF83-3E8B-4694-B8B1-96DCF6C6271E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BBE610F-FD71-401D-9DCE-6AF9F6A4B4C0}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="109">
   <si>
     <t>Имя файла</t>
   </si>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t>ZZZ.board</t>
+  </si>
+  <si>
+    <t>ERRORERROR.board</t>
+  </si>
+  <si>
+    <t>errorerrorerror.board</t>
+  </si>
+  <si>
+    <t>Колличество шагов13</t>
   </si>
 </sst>
 </file>
@@ -371,7 +380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,8 +423,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -436,11 +451,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -450,6 +476,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -519,8 +554,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36A937A9-4F5B-4971-9C8B-F8AF71BEB352}" name="Таблица1" displayName="Таблица1" ref="A1:K45" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:K45" xr:uid="{36A937A9-4F5B-4971-9C8B-F8AF71BEB352}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36A937A9-4F5B-4971-9C8B-F8AF71BEB352}" name="Таблица1" displayName="Таблица1" ref="A1:K47" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:K47" xr:uid="{36A937A9-4F5B-4971-9C8B-F8AF71BEB352}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{1CE8E175-F361-4C49-8FC0-D0643325FE40}" uniqueName="Имя файла" name="Имя файла">
       <xmlColumnPr mapId="1" xpath="/DocumentElement/results/Имя_x005f_x0020_файла" xmlDataType="string"/>
@@ -859,26 +894,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -918,8 +953,11 @@
       <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -959,8 +997,11 @@
       <c r="M2" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1000,8 +1041,11 @@
       <c r="M3" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -1021,8 +1065,11 @@
       <c r="M4" s="5">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="13">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1062,8 +1109,11 @@
       <c r="M5" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1103,8 +1153,11 @@
       <c r="M6" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1144,8 +1197,11 @@
       <c r="M7" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1185,8 +1241,11 @@
       <c r="M8" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1226,8 +1285,11 @@
       <c r="M9" s="6">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1267,8 +1329,11 @@
       <c r="M10" s="3">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1308,8 +1373,11 @@
       <c r="M11" s="4">
         <v>413</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="11">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1349,8 +1417,11 @@
       <c r="M12" s="3">
         <v>155</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="10">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1390,8 +1461,11 @@
       <c r="M13" s="4">
         <v>147</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="11">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1431,8 +1505,11 @@
       <c r="M14" s="5">
         <v>434</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="14">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1472,8 +1549,11 @@
       <c r="M15" s="4">
         <v>128</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1513,8 +1593,11 @@
       <c r="M16" s="3">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1554,8 +1637,11 @@
       <c r="M17" s="6">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="11">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1595,8 +1681,11 @@
       <c r="M18" s="3">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -1630,8 +1719,11 @@
       <c r="M19" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -1665,8 +1757,11 @@
       <c r="M20" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1706,8 +1801,11 @@
       <c r="M21" s="4">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1747,8 +1845,11 @@
       <c r="M22" s="3">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1788,8 +1889,11 @@
       <c r="M23" s="4">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="11">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1829,8 +1933,11 @@
       <c r="M24" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1870,8 +1977,11 @@
       <c r="M25" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1911,8 +2021,11 @@
       <c r="M26" s="3">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1952,8 +2065,11 @@
       <c r="M27" s="4">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1993,8 +2109,11 @@
       <c r="M28" s="3">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="10">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2034,628 +2153,761 @@
       <c r="M29" s="8">
         <v>73</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N30" s="10">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N31" s="12">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1" t="s">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K30">
+      <c r="K32">
         <v>105</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L32" s="3">
         <v>105</v>
       </c>
-      <c r="M30" s="3">
+      <c r="M32" s="3">
         <v>105</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="N32" s="10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C31">
+      <c r="C33">
         <v>102</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K31">
+      <c r="K33">
         <v>102</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L33" s="4">
         <v>102</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M33" s="4">
         <v>102</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="N33" s="11">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C32">
+      <c r="C34">
         <v>16</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K32">
+      <c r="K34">
         <v>16</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L34" s="3">
         <v>16</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M34" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="N34" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <v>13</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K33">
+      <c r="K35">
         <v>13</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L35" s="4">
         <v>17</v>
       </c>
-      <c r="M33" s="6">
+      <c r="M35" s="6">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="N35" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C34">
+      <c r="C36">
         <v>13</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K34">
+      <c r="K36">
         <v>13</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L36" s="3">
         <v>17</v>
       </c>
-      <c r="M34" s="7">
+      <c r="M36" s="7">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="N36" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C35">
+      <c r="C37">
         <v>16</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K35">
+      <c r="K37">
         <v>16</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L37" s="4">
         <v>20</v>
       </c>
-      <c r="M35" s="6">
+      <c r="M37" s="6">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="N37" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C36">
+      <c r="C38">
         <v>16</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K36">
+      <c r="K38">
         <v>16</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L38" s="3">
         <v>20</v>
       </c>
-      <c r="M36" s="7">
+      <c r="M38" s="7">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="N38" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C37">
+      <c r="C39">
         <v>18</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K37">
+      <c r="K39">
         <v>18</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L39" s="4">
         <v>22</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M39" s="6">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="N39" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C38">
+      <c r="C40">
         <v>18</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K38">
+      <c r="K40">
         <v>18</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L40" s="3">
         <v>22</v>
       </c>
-      <c r="M38" s="7">
+      <c r="M40" s="7">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="N40" s="10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C39">
+      <c r="C41">
         <v>20</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K39">
+      <c r="K41">
         <v>20</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L41" s="4">
         <v>20</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M41" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="N41" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <v>6</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K40">
+      <c r="K42">
         <v>6</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L42" s="3">
         <v>6</v>
       </c>
-      <c r="M40" s="3">
+      <c r="M42" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="N42" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C41">
+      <c r="C43">
         <v>10</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K41">
+      <c r="K43">
         <v>10</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L43" s="4">
         <v>10</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M43" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="N43" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C42">
+      <c r="C44">
         <v>16</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K42">
+      <c r="K44">
         <v>12</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L44" s="3">
         <v>12</v>
       </c>
-      <c r="M42" s="3">
+      <c r="M44" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="N44" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C43">
+      <c r="C45">
         <v>22</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K43">
+      <c r="K45">
         <v>15</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L45" s="4">
         <v>15</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M45" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="N45" s="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="3">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="3">
         <v>27</v>
       </c>
-      <c r="M44" s="7">
+      <c r="M46" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="N46" s="10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C45">
+      <c r="C47">
         <v>27</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K47" s="1">
         <v>27</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L47" s="4">
         <v>27</v>
       </c>
-      <c r="M45" s="4">
+      <c r="M47" s="4">
         <v>27</v>
       </c>
+      <c r="N47" s="11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new correct work with was_near_end
</commit_message>
<xml_diff>
--- a/Information/Изменение результатов.xlsx
+++ b/Information/Изменение результатов.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\MAPF_System\Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E86DF83-3E8B-4694-B8B1-96DCF6C6271E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001C04FE-D7F3-4B54-AC14-91A9C97B4C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BBE610F-FD71-401D-9DCE-6AF9F6A4B4C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="599" xr2:uid="{0BBE610F-FD71-401D-9DCE-6AF9F6A4B4C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -28,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="110">
   <si>
     <t>Имя файла</t>
   </si>
@@ -355,6 +368,9 @@
   </si>
   <si>
     <t>Колличество шагов13</t>
+  </si>
+  <si>
+    <t>ERROR_0.board</t>
   </si>
 </sst>
 </file>
@@ -380,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +445,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -466,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -484,7 +506,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -554,8 +585,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36A937A9-4F5B-4971-9C8B-F8AF71BEB352}" name="Таблица1" displayName="Таблица1" ref="A1:K47" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:K47" xr:uid="{36A937A9-4F5B-4971-9C8B-F8AF71BEB352}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36A937A9-4F5B-4971-9C8B-F8AF71BEB352}" name="Таблица1" displayName="Таблица1" ref="A1:K48" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:K48" xr:uid="{36A937A9-4F5B-4971-9C8B-F8AF71BEB352}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{1CE8E175-F361-4C49-8FC0-D0643325FE40}" uniqueName="Имя файла" name="Имя файла">
       <xmlColumnPr mapId="1" xpath="/DocumentElement/results/Имя_x005f_x0020_файла" xmlDataType="string"/>
@@ -894,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="R43" sqref="R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,9 +942,10 @@
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="17" max="23" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -956,8 +988,12 @@
       <c r="N1" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1000,8 +1036,19 @@
       <c r="N2" s="10">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="20">
+        <v>7</v>
+      </c>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1044,8 +1091,19 @@
       <c r="N3" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="20">
+        <v>3</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -1068,8 +1126,19 @@
       <c r="N4" s="13">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="22">
+        <v>43</v>
+      </c>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1112,8 +1181,19 @@
       <c r="N5" s="11">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="20">
+        <v>22</v>
+      </c>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1156,8 +1236,19 @@
       <c r="N6" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="20">
+        <v>3</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1200,8 +1291,19 @@
       <c r="N7" s="11">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="20">
+        <v>8</v>
+      </c>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1244,8 +1346,19 @@
       <c r="N8" s="10">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="20">
+        <v>15</v>
+      </c>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1288,8 +1401,19 @@
       <c r="N9" s="11">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="20">
+        <v>74</v>
+      </c>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1332,8 +1456,19 @@
       <c r="N10" s="10">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="20">
+        <v>67</v>
+      </c>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1376,8 +1511,19 @@
       <c r="N11" s="11">
         <v>413</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="20">
+        <v>413</v>
+      </c>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1420,8 +1566,19 @@
       <c r="N12" s="10">
         <v>155</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="20">
+        <v>155</v>
+      </c>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1464,8 +1621,19 @@
       <c r="N13" s="11">
         <v>147</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="20">
+        <v>147</v>
+      </c>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1508,8 +1676,19 @@
       <c r="N14" s="14">
         <v>337</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="23">
+        <v>461</v>
+      </c>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1552,8 +1731,19 @@
       <c r="N15" s="11">
         <v>128</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="20">
+        <v>128</v>
+      </c>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1596,8 +1786,19 @@
       <c r="N16" s="10">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="20">
+        <v>49</v>
+      </c>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1640,8 +1841,19 @@
       <c r="N17" s="11">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="20">
+        <v>68</v>
+      </c>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1684,8 +1896,19 @@
       <c r="N18" s="10">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="20">
+        <v>62</v>
+      </c>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -1722,8 +1945,19 @@
       <c r="N19" s="11">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="20">
+        <v>50</v>
+      </c>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -1760,8 +1994,19 @@
       <c r="N20" s="10">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="20">
+        <v>50</v>
+      </c>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1804,8 +2049,19 @@
       <c r="N21" s="11">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="20">
+        <v>48</v>
+      </c>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1848,8 +2104,19 @@
       <c r="N22" s="10">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="20">
+        <v>43</v>
+      </c>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1892,8 +2159,19 @@
       <c r="N23" s="11">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="20">
+        <v>96</v>
+      </c>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1936,8 +2214,19 @@
       <c r="N24" s="10">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="20">
+        <v>18</v>
+      </c>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1980,8 +2269,19 @@
       <c r="N25" s="11">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="20">
+        <v>15</v>
+      </c>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2024,8 +2324,19 @@
       <c r="N26" s="10">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="20">
+        <v>51</v>
+      </c>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -2068,8 +2379,19 @@
       <c r="N27" s="11">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="20">
+        <v>32</v>
+      </c>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="20"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2112,8 +2434,19 @@
       <c r="N28" s="10">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="20">
+        <v>69</v>
+      </c>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2156,8 +2489,19 @@
       <c r="N29" s="15">
         <v>66</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="23">
+        <v>72</v>
+      </c>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="20"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>106</v>
       </c>
@@ -2167,8 +2511,19 @@
       <c r="N30" s="10">
         <v>122</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="22">
+        <v>106</v>
+      </c>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="20"/>
+      <c r="T30" s="20"/>
+      <c r="U30" s="20"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>107</v>
       </c>
@@ -2178,174 +2533,193 @@
       <c r="N31" s="12">
         <v>413</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="23">
+        <v>430</v>
+      </c>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N32" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1" t="s">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K32">
+      <c r="K33">
         <v>105</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L33" s="3">
         <v>105</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M33" s="3">
         <v>105</v>
       </c>
-      <c r="N32" s="10">
+      <c r="N33" s="10">
         <v>105</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="O33" s="20">
+        <v>105</v>
+      </c>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>102</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K33">
+      <c r="K34">
         <v>102</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L34" s="4">
         <v>102</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M34" s="4">
         <v>102</v>
       </c>
-      <c r="N33" s="11">
+      <c r="N34" s="11">
         <v>102</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="O34" s="20">
+        <v>102</v>
+      </c>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>16</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K34">
+      <c r="K35">
         <v>16</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L35" s="3">
         <v>16</v>
       </c>
-      <c r="M34" s="3">
+      <c r="M35" s="3">
         <v>16</v>
       </c>
-      <c r="N34" s="10">
+      <c r="N35" s="10">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="O35" s="20">
+        <v>16</v>
+      </c>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35">
-        <v>13</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K35">
-        <v>13</v>
-      </c>
-      <c r="L35" s="4">
-        <v>17</v>
-      </c>
-      <c r="M35" s="6">
-        <v>13</v>
-      </c>
-      <c r="N35" s="11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>61</v>
@@ -2377,63 +2751,85 @@
       <c r="K36">
         <v>13</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36" s="4">
         <v>17</v>
       </c>
-      <c r="M36" s="7">
+      <c r="M36" s="6">
         <v>13</v>
       </c>
-      <c r="N36" s="10">
+      <c r="N36" s="11">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="20">
+        <v>13</v>
+      </c>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K37">
+        <v>13</v>
+      </c>
+      <c r="L37" s="3">
+        <v>17</v>
+      </c>
+      <c r="M37" s="7">
+        <v>13</v>
+      </c>
+      <c r="N37" s="10">
+        <v>13</v>
+      </c>
+      <c r="O37" s="20">
+        <v>13</v>
+      </c>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37">
-        <v>16</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K37">
-        <v>16</v>
-      </c>
-      <c r="L37" s="4">
-        <v>20</v>
-      </c>
-      <c r="M37" s="6">
-        <v>16</v>
-      </c>
-      <c r="N37" s="11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>46</v>
@@ -2465,63 +2861,85 @@
       <c r="K38">
         <v>16</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="4">
         <v>20</v>
       </c>
-      <c r="M38" s="7">
+      <c r="M38" s="6">
         <v>16</v>
       </c>
-      <c r="N38" s="10">
+      <c r="N38" s="11">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="20">
+        <v>16</v>
+      </c>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39">
+        <v>16</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K39">
+        <v>16</v>
+      </c>
+      <c r="L39" s="3">
+        <v>20</v>
+      </c>
+      <c r="M39" s="7">
+        <v>16</v>
+      </c>
+      <c r="N39" s="10">
+        <v>16</v>
+      </c>
+      <c r="O39" s="20">
+        <v>16</v>
+      </c>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39">
-        <v>18</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K39">
-        <v>18</v>
-      </c>
-      <c r="L39" s="4">
-        <v>22</v>
-      </c>
-      <c r="M39" s="6">
-        <v>18</v>
-      </c>
-      <c r="N39" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>56</v>
@@ -2553,313 +2971,446 @@
       <c r="K40">
         <v>18</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40" s="4">
         <v>22</v>
       </c>
-      <c r="M40" s="7">
+      <c r="M40" s="6">
         <v>18</v>
       </c>
-      <c r="N40" s="10">
+      <c r="N40" s="11">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="20">
+        <v>18</v>
+      </c>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K41">
+        <v>18</v>
+      </c>
+      <c r="L41" s="3">
+        <v>22</v>
+      </c>
+      <c r="M41" s="7">
+        <v>18</v>
+      </c>
+      <c r="N41" s="10">
+        <v>18</v>
+      </c>
+      <c r="O41" s="20">
+        <v>18</v>
+      </c>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="20"/>
+      <c r="T41" s="20"/>
+      <c r="U41" s="20"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>20</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K41">
+      <c r="K42">
         <v>20</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L42" s="4">
         <v>20</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M42" s="4">
         <v>20</v>
       </c>
-      <c r="N41" s="11">
+      <c r="N42" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="O42" s="20">
+        <v>20</v>
+      </c>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>6</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K42">
+      <c r="K43">
         <v>6</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L43" s="3">
         <v>6</v>
       </c>
-      <c r="M42" s="3">
+      <c r="M43" s="3">
         <v>6</v>
       </c>
-      <c r="N42" s="10">
+      <c r="N43" s="10">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="O43" s="20">
+        <v>6</v>
+      </c>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>10</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K43">
+      <c r="K44">
         <v>10</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L44" s="4">
         <v>10</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M44" s="4">
         <v>10</v>
       </c>
-      <c r="N43" s="11">
+      <c r="N44" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="O44" s="20">
+        <v>10</v>
+      </c>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>16</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K44">
+      <c r="K45">
         <v>12</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L45" s="3">
         <v>12</v>
       </c>
-      <c r="M44" s="3">
+      <c r="M45" s="3">
         <v>12</v>
       </c>
-      <c r="N44" s="10">
+      <c r="N45" s="10">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="O45" s="20">
+        <v>12</v>
+      </c>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="20"/>
+      <c r="S45" s="20"/>
+      <c r="T45" s="20"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>22</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K45">
+      <c r="K46">
         <v>15</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L46" s="4">
         <v>15</v>
       </c>
-      <c r="M45" s="4">
+      <c r="M46" s="4">
         <v>15</v>
       </c>
-      <c r="N45" s="16">
+      <c r="N46" s="16">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="O46" s="22">
+        <v>22</v>
+      </c>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="20"/>
+      <c r="S46" s="26"/>
+      <c r="T46" s="26"/>
+      <c r="U46" s="20"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="3">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="3">
         <v>27</v>
       </c>
-      <c r="M46" s="7">
+      <c r="M47" s="7">
         <v>23</v>
       </c>
-      <c r="N46" s="10">
+      <c r="N47" s="10">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="O47" s="20">
+        <v>23</v>
+      </c>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="20"/>
+      <c r="T47" s="20"/>
+      <c r="U47" s="20"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>27</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K48" s="1">
         <v>27</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L48" s="4">
         <v>27</v>
       </c>
-      <c r="M47" s="4">
+      <c r="M48" s="4">
         <v>27</v>
       </c>
-      <c r="N47" s="11">
+      <c r="N48" s="11">
         <v>27</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O48" s="20">
+        <v>27</v>
+      </c>
+      <c r="P48" s="21"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="20"/>
+      <c r="T48" s="20"/>
+      <c r="U48" s="20"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+    </row>
+    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2869,7 +3420,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2878,8 +3429,16 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <f>SUM((N2:N30,N31,N33:N48))</f>
+        <v>3123</v>
+      </c>
+      <c r="O50">
+        <f>SUM((O2:O30,O31,O33:O48))</f>
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2889,7 +3448,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2899,7 +3458,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>

</xml_diff>